<commit_message>
update user input template
</commit_message>
<xml_diff>
--- a/Template/input_template.xlsx
+++ b/Template/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelfive/Desktop/R Directory/Git learning/MR-automation/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1558A51B-FA3B-7548-8F04-405FD1BF736F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23631ADB-1AC4-454E-8D02-E66FD8887E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
+    <workbookView xWindow="-38380" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27BFF5F-7205-9748-9F48-9C16FDA3EB73}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,9 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4276D3E0-CD11-5045-8B57-1997DA2EBF68}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
+    <sheetView zoomScale="174" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1095,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601705C5-50A2-7A46-BFF2-1E1E17DB5A98}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="209" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
extract eigenvalues and add EFA screeplot
</commit_message>
<xml_diff>
--- a/Template/input_template.xlsx
+++ b/Template/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelfive/Desktop/R Directory/Git learning/MR-automation/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D8D5C0-D5ED-214F-9724-CE36E079FD9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CD77D-EBA8-5941-B855-7E35EA2E44E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>model_file_path</t>
   </si>
@@ -420,6 +420,18 @@
   </si>
   <si>
     <t>~/Box/For Zezhen/MR automation/Test Data</t>
+  </si>
+  <si>
+    <t>model_efa</t>
+  </si>
+  <si>
+    <t>CS1_EFA.out</t>
+  </si>
+  <si>
+    <t>CS2_EFA.out</t>
+  </si>
+  <si>
+    <t>CS3_EFA.out</t>
   </si>
 </sst>
 </file>
@@ -773,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27BFF5F-7205-9748-9F48-9C16FDA3EB73}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
+    <sheetView zoomScale="192" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1091,152 +1103,164 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601705C5-50A2-7A46-BFF2-1E1E17DB5A98}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="209" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D10"/>
+    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>115</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>98</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>116</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>99</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>117</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>109</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>110</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>102</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>111</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>103</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>112</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>113</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>114</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>